<commit_message>
CCDI - Strip CPI mappings from Participant IDs column, update TC01 for phs000466
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs000466_SexAtBirth-Male.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs000466_SexAtBirth-Male.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/03-28-2025/Commons_Automation/InputFiles/CCDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git2/Commons_Automation/InputFiles/CCDI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08830B4-CE9A-884B-BC38-D2DC44B1316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5E603-EB0E-DC42-83BE-555F69E59F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-3680" windowWidth="51200" windowHeight="28300" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="35080" windowHeight="22500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,56 +63,6 @@
   </si>
   <si>
     <t>StudiesTab</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT std.dbgap_accession) AS "Studies",
-    COUNT(DISTINCT prt.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    (COUNT(DISTINCT cmf.id)) AS "Files"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_clinical_measure_file cmf ON std.id = cmf."study.id"
-WHERE 
-    std.dbgap_accession = 'phs000466' AND prt.sex_at_birth = 'Male';</t>
-  </si>
-  <si>
-    <t>with diagnosis1 as (
-select dgn."participant.id", group_concat(dgn.age_at_diagnosis,';') as age, group_concat(dgn.diagnosis,';') as diag,group_concat(dgn.anatomic_site,';') as ant_site from df_diagnosis dgn where dgn."participant.id" is not null group by dgn."participant.id" ),
-diagnosis2 as (select "participant.id",  group_concat(diagnosis,';') as diag from (select distinct "participant.id", diagnosis from df_diagnosis  where "participant.id" is not null )  group by "participant.id" ),
-diagnosis3 as (select "participant.id",  group_concat(anatomic_site,';') as ant_site from (select distinct "participant.id", anatomic_site from df_diagnosis where "participant.id" is not null ) group by "participant.id" ) 
-SELECT DISTINCT
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    COALESCE(prt.sex_at_birth, '') AS "Sex",
-    COALESCE(prt.race, '') AS "Race",
-	dgn2.diag AS "Diagnosis",
-	dgn3.ant_site AS "Diagnosis Anatomic Site",
-	   COALESCE(CASE WHEN dgn1.age = '-999' THEN 'Not Reported' ELSE dgn1.age END, "") AS "Age at Diagnosis (days)",
-	null AS "Treatment Type",
-	srv.last_known_survival_status AS "Last Known Survival Status"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    diagnosis1 dgn1 ON prt.id = dgn1."participant.id" 
-LEFT JOIN 
-    diagnosis2 dgn2 ON prt.id = dgn2."participant.id"
-LEFT JOIN 
-    diagnosis3 dgn3 ON prt.id = dgn3."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-WHERE 
-    std.dbgap_accession = 'phs000466' AND prt.sex_at_birth = 'Male'
-ORDER BY 
-    prt.participant_id ASC 
-;</t>
   </si>
   <si>
     <t>WITH Study AS (
@@ -232,98 +182,235 @@
 LEFT JOIN funding fd ON s.study_id = fd.study_id;  -- Changed alias from 'f' to 'fd' here</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    prt.participant_id AS "Participant ID",
-    std.dbgap_accession AS "Study ID",
-    smp.anatomic_site AS "Sample Anatomic Site",
+    <t>TC01_CCDI_phs000466_SexAtBirth-Male_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_CCDI_phs000466_SexAtBirth-Male_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>WITH diagnosis1 AS (
+  SELECT
+      dgn."participant.id" AS pid,
+      group_concat(
+        CASE WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported'
+             ELSE CAST(dgn.age_at_diagnosis AS VARCHAR) END, ', '
+      ) AS age
+  FROM df_diagnosis dgn
+  WHERE dgn."participant.id" IS NOT NULL
+  GROUP BY dgn."participant.id"
+),
+diagnosis2 AS (
+  SELECT
+      dgn."participant.id" AS pid,
+      group_concat(dgn.diagnosis, ', ') AS diag
+  FROM df_diagnosis dgn
+  WHERE dgn."participant.id" IS NOT NULL
+  GROUP BY dgn."participant.id"
+),
+diagnosis3 AS (
+  SELECT
+      dgn."participant.id" AS pid,
+      group_concat(dgn.anatomic_site, ', ') AS ant_site
+  FROM df_diagnosis dgn
+  WHERE dgn."participant.id" IS NOT NULL
+  GROUP BY dgn."participant.id"
+),
+diagnosis4 AS (
+  SELECT
+      dgn."participant.id" AS pid,
+      group_concat(dgn.diagnosis_category, ', ') AS diag_cat
+  FROM df_diagnosis dgn
+  WHERE dgn."participant.id" IS NOT NULL
+  GROUP BY dgn."participant.id"
+)
+SELECT DISTINCT
+    prt.participant_id                 AS "Participant ID",
+    std.dbgap_accession                AS "Study ID",
+    COALESCE(prt.sex_at_birth, '')     AS "Sex",
+    COALESCE(prt.race, '')             AS "Race",
+    d2.diag                            AS "Diagnosis",
+    d3.ant_site                        AS "Diagnosis Anatomic Site",
+    d4.diag_cat                        AS "Diagnosis Category",
+    COALESCE(d1.age, '')               AS "Age at Diagnosis (days)",
+    NULL                               AS "Treatment Type",
+    srv.last_known_survival_status     AS "Last Known Survival Status"
+FROM df_study std
+JOIN df_consent_group cg
+  ON std.id = cg."study.id"
+JOIN df_participant prt
+  ON cg.id = prt."consent_group.id"
+LEFT JOIN diagnosis1 d1 ON prt.id = d1.pid
+LEFT JOIN diagnosis2 d2 ON prt.id = d2.pid
+LEFT JOIN diagnosis3 d3 ON prt.id = d3.pid
+LEFT JOIN diagnosis4 d4 ON prt.id = d4.pid
+LEFT JOIN df_survival  srv ON prt.id = srv."participant.id"
+WHERE
+    std.dbgap_accession = 'phs000466'
+    AND prt.sex_at_birth = 'Male'
+ORDER BY prt.participant_id ASC;</t>
+  </si>
+  <si>
+    <t>SELECT
+  s.Studies,
+  p.Participants,
+  sa.Samples,
+  f.Files
+FROM
+  -- Studies (by accession)
+  ( SELECT COUNT(DISTINCT std.dbgap_accession) AS Studies
+    FROM df_study std
+    WHERE std.dbgap_accession = 'phs000466'
+  ) s
+CROSS JOIN
+  -- Participants (Male)
+  ( SELECT COUNT(DISTINCT prt.participant_id) AS Participants
+    FROM df_study std
+    JOIN df_consent_group cg ON std.id = cg."study.id"
+    JOIN df_participant prt  ON cg.id  = prt."consent_group.id"
+    WHERE std.dbgap_accession = 'phs000466'
+      AND prt.sex_at_birth = 'Male'
+  ) p
+CROSS JOIN
+  -- Samples (belonging to Male participants)
+  ( SELECT COUNT(DISTINCT smp.sample_id) AS Samples
+    FROM df_study std
+    JOIN df_consent_group cg ON std.id = cg."study.id"
+    JOIN df_participant prt  ON cg.id  = prt."consent_group.id"
+    LEFT JOIN df_sample smp  ON prt.id = smp."participant.id"
+    WHERE std.dbgap_accession = 'phs000466'
+      AND prt.sex_at_birth = 'Male'
+  ) sa
+CROSS JOIN
+  -- Files: count study-level clinical files for this accession (ignore participant filter)
+  ( SELECT COUNT(DISTINCT cmf.id) AS Files
+    FROM df_clinical_measure_file cmf
+    JOIN df_study std2 ON cmf."study.id" = std2.id
+    WHERE std2.dbgap_accession = 'phs000466'
+          -- If your engine stores missing participant IDs as empty strings, this still counts them
+          -- (no WHERE on participant.id at all, because these are study-level files)
+  ) f;</t>
+  </si>
+  <si>
+    <t>WITH sample_dx AS (
+    SELECT
+        dgn."sample.id" AS sid,
+        GROUP_CONCAT(dgn.diagnosis, ', ')          AS diag,
+        GROUP_CONCAT(dgn.diagnosis_category, ', ') AS diag_cat
+    FROM df_diagnosis dgn
+    WHERE dgn."sample.id" IS NOT NULL
+    GROUP BY dgn."sample.id"
+)
+SELECT DISTINCT
+    smp.sample_id                                AS "Sample ID",
+    prt.participant_id                           AS "Participant ID",
+    std.dbgap_accession                          AS "Study ID",
+    COALESCE(smp.anatomic_site, '')              AS "Sample Anatomic Site",
     COALESCE(
-        CASE 
-            WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' 
-            ELSE smp.participant_age_at_collection 
-        END, 
-        0
-    ) AS "Age at Sample Collection (days)",
-    COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
-    COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification",
-    dgn.diagnosis AS "Sample Diagnosis"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_sample smp ON prt.id = smp."participant.id"
-LEFT JOIN 
-    df_diagnosis dgn ON smp.id = dgn."sample.id"
-WHERE 
-    std.dbgap_accession = 'phs000466' 
+      CASE
+        WHEN smp.participant_age_at_collection = -999
+          THEN 'Not Reported'
+        ELSE CAST(smp.participant_age_at_collection AS VARCHAR)
+      END,
+      'Not Reported'
+    )                                            AS "Age at Sample Collection (days)",
+    COALESCE(smp.sample_tumor_status, '')        AS "Sample Tumor Status",
+    COALESCE(smp.tumor_classification, '')       AS "Sample Tumor Classification",
+    sdx.diag                                     AS "Sample Diagnosis",
+    sdx.diag_cat                                 AS "Diagnosis Category"
+FROM df_study std
+JOIN df_consent_group cg
+  ON std.id = cg."study.id"
+JOIN df_participant prt
+  ON cg.id = prt."consent_group.id"
+LEFT JOIN df_sample smp
+  ON prt.id = smp."participant.id"
+LEFT JOIN sample_dx sdx
+  ON smp.id = sdx.sid
+WHERE
+    std.dbgap_accession = 'phs000466'
     AND prt.sex_at_birth = 'Male'
     AND smp.sample_id IS NOT NULL
-ORDER BY 
+ORDER BY
     smp.sample_id ASC;</t>
   </si>
   <si>
-    <t>with file_data as (
-select file_name, data_category, file_type, file_size, file_access, file_description,"study.id" studyid, "participant.id" as participantid from df_clinical_measure_file )
-SELECT fd.file_name AS "File Name",
-    fd.data_category AS "Data Category",
-    COALESCE(fd.file_description, '') AS "File Description",
-    fd.file_type AS "File Type" ,
-        CASE     
-    WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
-        END
-    WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
-            ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
-        END
-    WHEN fd.file_size &gt;= 1024 THEN 
-        CASE 
-            WHEN ROUND(fd.file_size / 1024.0, 2) = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
-            ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
-        END
-    ELSE 
-        CASE 
-            WHEN ROUND(fd.file_size, 2) = CAST(ROUND(fd.file_size, 0) AS INT) 
-            THEN CAST(CAST(ROUND(fd.file_size, 0) AS INT) AS TEXT) || ' Bytes'
-            ELSE ROUND(fd.file_size, 2) || ' Bytes'
-        END
-END AS "File Size",
-fd.file_access AS "File Access", std.dbgap_accession AS "Study ID", fd.participantid AS "Participant ID", null as "Sample ID"
-FROM 
-    df_study std
- LEFT JOIN  
-    file_data fd ON std.id = fd.studyid
-WHERE 
-    std.dbgap_accession = 'phs000466'</t>
-  </si>
-  <si>
-    <t>TC01_CCDI_phs000466_SexAtBirth-Male_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_CCDI_phs000466_SexAtBirth-Male_WebData.xlsx</t>
+    <t>WITH file_data AS (
+  SELECT
+    cmf.file_name,
+    REPLACE(COALESCE(cmf.data_category, ''), ';', ', ') AS data_category,
+    COALESCE(cmf.file_description, '')                  AS file_description,
+    cmf.file_type,
+    cmf.file_access,
+    cmf.file_size,
+    cmf."study.id"        AS study_row_id,
+    cmf."participant.id"  AS participant_row_id
+  FROM df_clinical_measure_file cmf
+)
+SELECT DISTINCT
+  fd.file_name                               AS "File Name",
+  fd.data_category                           AS "Data Category",
+  fd.file_description                        AS "File Description",
+  fd.file_type                               AS "File Type",
+  CASE
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2)
+             = CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 * 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / (1024.0 * 1024.0), 2)
+             = CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+        ELSE ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB'
+      END
+    WHEN COALESCE(fd.file_size, 0) &gt;= 1024 THEN
+      CASE
+        WHEN ROUND(fd.file_size / 1024.0, 2)
+             = CAST(ROUND(fd.file_size / 1024.0, 0) AS INT)
+        THEN CAST(CAST(ROUND(fd.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+        ELSE ROUND(fd.file_size / 1024.0, 2) || ' KB'
+      END
+    ELSE
+      CASE
+        WHEN ROUND(COALESCE(fd.file_size, 0), 2)
+             = CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT)
+        THEN CAST(CAST(ROUND(COALESCE(fd.file_size, 0), 0) AS INT) AS TEXT) || ' Bytes'
+        ELSE ROUND(COALESCE(fd.file_size, 0), 2) || ' Bytes'
+      END
+  END                                         AS "File Size",
+  fd.file_access                              AS "File Access",
+  std.dbgap_accession                         AS "Study ID",
+  COALESCE(prt.participant_id, '')            AS "Participant ID",
+  ''                                          AS "Sample ID"   -- still not sample-level
+FROM df_study std
+JOIN file_data fd
+  ON std.id = fd.study_row_id
+LEFT JOIN df_participant prt
+  ON prt.id = fd.participant_row_id
+WHERE
+    std.dbgap_accession = 'phs000466'
+    AND (
+         -- include study-level files (no participant or blank)
+         fd.participant_row_id IS NULL
+         OR TRIM(COALESCE(fd.participant_row_id, '')) = ''
+         -- OR participant-linked Male (future-proof)
+         OR prt.sex_at_birth = 'Male'
+    )
+ORDER BY
+  fd.file_name
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -390,17 +477,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -729,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -762,25 +846,25 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -789,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -798,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -809,7 +893,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>